<commit_message>
Novo método para fazer MergeExcel
</commit_message>
<xml_diff>
--- a/AppExcel/Planilhas/Despesas1.xlsx
+++ b/AppExcel/Planilhas/Despesas1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Wagner\Desktop\Gerar e Ler Excel\AppExcel\AppExcel\Planilhas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Wagner\Desktop\POCs\ExcelClosedXml\AppExcel\AppExcel\Planilhas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5939178-2367-41DC-96B0-5FCEA24A0E9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{452582AC-EF20-40BA-B971-8FBCD34D6A41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="2505" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Despesas" sheetId="2" r:id="rId1"/>

</xml_diff>